<commit_message>
alkylating agents and NCI update
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharma_oncox.xlsx
+++ b/data-raw/metadata_pharma_oncox.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__oncoPharmaDB/oncoPharmaDB/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__pharmaOncoX/pharmaOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE3BAFB-FA80-F94C-9552-27B817BD34AD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC01B1CC-97A9-D342-B26F-0F12DF3E97C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="10900" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
+    <workbookView xWindow="6360" yWindow="5200" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="compounds" sheetId="2" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>v2022_02</t>
   </si>
   <si>
-    <t>22.07d</t>
-  </si>
-  <si>
     <t>PubChem</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>https://depmap.org/repurposing/</t>
+  </si>
+  <si>
+    <t>22.08e</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -647,7 +647,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -667,10 +667,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -687,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -698,19 +698,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -767,93 +767,93 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
         <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
         <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NCI & OT update, fixed 0.9.7 bug
</commit_message>
<xml_diff>
--- a/data-raw/metadata_pharma_oncox.xlsx
+++ b/data-raw/metadata_pharma_oncox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sigven/project_data/package__pharmaOncoX/pharmaOncoX/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC01B1CC-97A9-D342-B26F-0F12DF3E97C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA9C3E0-C2AD-284D-9052-308E2DCF759D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="5200" windowWidth="26840" windowHeight="15940" xr2:uid="{FE925BBA-8697-304B-A498-CFC01A1CEF4E}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>https://www.dgidb.org</t>
   </si>
   <si>
-    <t>2022.06</t>
-  </si>
-  <si>
     <t>opentargets</t>
   </si>
   <si>
@@ -196,7 +193,10 @@
     <t>https://depmap.org/repurposing/</t>
   </si>
   <si>
-    <t>22.08e</t>
+    <t>22.09d</t>
+  </si>
+  <si>
+    <t>2022.09</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CAA087-5CE9-5744-85B8-F0D7703C76D2}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -647,13 +647,13 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -667,13 +667,13 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -687,30 +687,30 @@
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -767,93 +767,93 @@
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
         <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>